<commit_message>
add plant to guild analysis
</commit_message>
<xml_diff>
--- a/rawdata/Iva_plant_sample.xlsx
+++ b/rawdata/Iva_plant_sample.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
@@ -261,208 +261,7 @@
     <cellStyle name="Normal 2" xfId="1"/>
     <cellStyle name="一般" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="20">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -775,10 +574,10 @@
   <dimension ref="A1:V360"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="8" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="8" ySplit="1" topLeftCell="I347" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="V1" sqref="V1"/>
+      <selection pane="bottomRight" activeCell="U165" sqref="U165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -7788,7 +7587,7 @@
         <v>1</v>
       </c>
       <c r="M108" s="3">
-        <v>12</v>
+        <v>120</v>
       </c>
       <c r="N108" s="3">
         <v>80</v>
@@ -10973,7 +10772,7 @@
         <v>1</v>
       </c>
       <c r="M157" s="3">
-        <v>10</v>
+        <v>180</v>
       </c>
       <c r="N157" s="3">
         <v>100</v>

</xml_diff>